<commit_message>
Executed TC for Registration v1.
</commit_message>
<xml_diff>
--- a/qa/Registration-mobAPP(Executed).xlsx
+++ b/qa/Registration-mobAPP(Executed).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="166">
   <si>
     <t>Project Name</t>
   </si>
@@ -143,17 +143,7 @@
     <t>R-009</t>
   </si>
   <si>
-    <t>1. GoTo Registration TC.
-2. Enter password with only uppercase letters.
-3. Run TC.</t>
-  </si>
-  <si>
     <t>R-010</t>
-  </si>
-  <si>
-    <t>1. GoTo Registration TC.
-2. Enter password with only lowercase letters.
-3. Run TC.</t>
   </si>
   <si>
     <t>Registration by authenticated user</t>
@@ -251,12 +241,6 @@
     <t xml:space="preserve">Registration-&gt; Password &lt;8 characters     </t>
   </si>
   <si>
-    <t xml:space="preserve">Registration-&gt; Password with only uppercase letters.     </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registration -&gt; Password with only lowercase letters.     </t>
-  </si>
-  <si>
     <t>1. GoTo Registration TC.
 2. Enter password &amp; all details.
 3. Run TC.</t>
@@ -378,10 +362,6 @@
   </si>
   <si>
     <t>Registration-&gt;gender field is missing</t>
-  </si>
-  <si>
-    <t>It successfully  added the values in DB and Verified.
-But need to get proper success message.</t>
   </si>
   <si>
     <t>Pass</t>
@@ -392,10 +372,6 @@
   <si>
     <t xml:space="preserve"> Error message,
 "All fields are mandatory"</t>
-  </si>
-  <si>
-    <t>Pass
-Bug- 0000003</t>
   </si>
   <si>
     <t>Expecting proper response message</t>
@@ -419,10 +395,6 @@
   </si>
   <si>
     <t>Pass
-Bug- 0000006</t>
-  </si>
-  <si>
-    <t>Pass
 Bug- 0000007</t>
   </si>
   <si>
@@ -440,10 +412,6 @@
   </si>
   <si>
     <t>Pass
-Bug- 0000008</t>
-  </si>
-  <si>
-    <t>Pass
 Bug- 0000009</t>
   </si>
   <si>
@@ -460,23 +428,11 @@
 </t>
   </si>
   <si>
-    <t>Pass
-Bug- 0000010</t>
-  </si>
-  <si>
-    <t>Fail
-Bug- 0000011</t>
-  </si>
-  <si>
     <t xml:space="preserve">Registration-&gt; Junk Password     </t>
   </si>
   <si>
     <t>Error message,
 "Password is not valid"</t>
-  </si>
-  <si>
-    <t>Fail
-Bug- 0000012</t>
   </si>
   <si>
     <t>Registration-&gt;Password with null value</t>
@@ -490,18 +446,6 @@
 </t>
   </si>
   <si>
-    <t>Pass
-Bug- 0000013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registration -&gt; Password with only numbers.     </t>
-  </si>
-  <si>
-    <t>1. GoTo Registration TC.
-2. Enter password with only numbers.
-3. Run TC.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Registration-&gt; Junk value in mobile     </t>
   </si>
   <si>
@@ -593,14 +537,6 @@
 </t>
   </si>
   <si>
-    <t>Fail
-Bug- 0000019</t>
-  </si>
-  <si>
-    <t>Pass
-Bug- 0000020</t>
-  </si>
-  <si>
     <t>R-035</t>
   </si>
   <si>
@@ -620,14 +556,6 @@
     <t>R-036</t>
   </si>
   <si>
-    <t>Fail
-Bug- 0000021</t>
-  </si>
-  <si>
-    <t>Pass
-Bug- 0000022</t>
-  </si>
-  <si>
     <t>R-037</t>
   </si>
   <si>
@@ -672,6 +600,49 @@
   <si>
     <t>Error message,
 "Gender type is not valid"</t>
+  </si>
+  <si>
+    <t>Fail
+Bug- 0000026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration-&gt; Password without uppercase letters.     </t>
+  </si>
+  <si>
+    <t>1. GoTo Registration TC.
+2. Enter password without uppercase letters.
+3. Run TC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration -&gt; Password without lowercase letters.     </t>
+  </si>
+  <si>
+    <t>1. GoTo Registration TC.
+2. Enter password without lowercase letters.
+3. Run TC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration -&gt; Password without number.     </t>
+  </si>
+  <si>
+    <t>1. GoTo Registration TC.
+2. Enter password without numbers.
+3. Run TC.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration -&gt; Password without special characters(@#$%).     </t>
+  </si>
+  <si>
+    <t>1. GoTo Registration TC.
+2. Enter password without special characters
+3. Run TC.</t>
+  </si>
+  <si>
+    <t>R-040</t>
   </si>
 </sst>
 </file>
@@ -825,7 +796,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -858,9 +829,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -876,6 +844,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1171,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1183,15 +1161,15 @@
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1240,33 +1218,39 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:6" s="20" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A6" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="10"/>
-    </row>
-    <row r="6" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
-      <c r="A6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="15" t="s">
+      <c r="D6" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>41</v>
+      <c r="E6" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="F6" s="11"/>
     </row>
@@ -1275,7 +1259,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>11</v>
@@ -1284,27 +1268,25 @@
         <v>12</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>97</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F8" s="10"/>
     </row>
@@ -1313,7 +1295,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>17</v>
@@ -1322,10 +1304,10 @@
         <v>18</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
@@ -1333,16 +1315,16 @@
         <v>25</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F10" s="11"/>
     </row>
@@ -1351,16 +1333,16 @@
         <v>28</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="F11" s="10"/>
     </row>
@@ -1369,7 +1351,7 @@
         <v>31</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>20</v>
@@ -1378,7 +1360,7 @@
         <v>21</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F12" s="10"/>
     </row>
@@ -1387,43 +1369,43 @@
         <v>32</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A14" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>112</v>
+        <v>156</v>
       </c>
       <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A15" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>22</v>
@@ -1432,476 +1414,490 @@
         <v>24</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A16" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" ht="42.75">
+      <c r="A18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" spans="1:6" ht="57">
-      <c r="A18" s="10" t="s">
-        <v>46</v>
-      </c>
       <c r="B18" s="8" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="71.25">
       <c r="A19" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>27</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A21" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6" ht="57">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="C22" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="57">
+      <c r="A23" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="57">
+      <c r="A24" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="57">
-      <c r="A23" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="57">
-      <c r="A24" s="13" t="s">
+      <c r="B24" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="57">
+      <c r="A25" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="57">
+      <c r="A26" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="57">
-      <c r="A25" s="13" t="s">
+      <c r="B26" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="57">
+      <c r="A27" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="57">
-      <c r="A26" s="10" t="s">
+      <c r="B27" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A28" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="E26" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
-      <c r="A27" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="16" t="s">
+      <c r="B28" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A29" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
-      <c r="A28" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="F28" s="10"/>
-    </row>
-    <row r="29" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
-      <c r="A29" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>130</v>
+      <c r="D29" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="F29" s="10"/>
     </row>
     <row r="30" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
-      <c r="A30" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>132</v>
+      <c r="A30" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="F30" s="10"/>
     </row>
     <row r="31" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A31" s="10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>134</v>
+        <v>49</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="F31" s="11"/>
+        <v>118</v>
+      </c>
+      <c r="F31" s="10"/>
     </row>
     <row r="32" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A32" s="10" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>136</v>
-      </c>
       <c r="E32" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="F32" s="10"/>
+        <v>127</v>
+      </c>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A33" s="10" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>143</v>
+        <v>70</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>122</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
-      <c r="A34" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="16" t="s">
+      <c r="A34" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A35" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A36" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A37" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D34" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F34" s="10"/>
-    </row>
-    <row r="35" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
-      <c r="A35" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F35" s="10"/>
-    </row>
-    <row r="36" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
-      <c r="A36" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D36" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="F36" s="10"/>
-    </row>
-    <row r="37" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
-      <c r="A37" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="F37" s="11"/>
+      <c r="D37" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F37" s="10"/>
     </row>
     <row r="38" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A38" s="10" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="B38" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="F38" s="10"/>
+      <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A39" s="10" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
       <c r="C39" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="F39" s="11"/>
+      <c r="F39" s="10"/>
     </row>
     <row r="40" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A40" s="10" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>73</v>
+        <v>140</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>157</v>
+        <v>95</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="F40" s="10"/>
+        <v>93</v>
+      </c>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A41" s="10" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>162</v>
+        <v>90</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>163</v>
+        <v>69</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>100</v>
+        <v>141</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="F41" s="11"/>
+        <v>156</v>
+      </c>
+      <c r="F41" s="10"/>
     </row>
     <row r="42" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A42" s="10" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>78</v>
+        <v>145</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>164</v>
+        <v>95</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="F42" s="10"/>
+        <v>147</v>
+      </c>
+      <c r="F42" s="11"/>
     </row>
     <row r="43" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
       <c r="A43" s="10" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>169</v>
+        <v>92</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>172</v>
+        <v>74</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>146</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="F43" s="10"/>
+    </row>
+    <row r="44" spans="1:6" s="9" customFormat="1" ht="90.75" customHeight="1">
+      <c r="A44" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="F44" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>